<commit_message>
Atualizado por script em 24-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/croatia_prva-nl_2023-2024.xlsx
+++ b/2023/croatia_prva-nl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Vukovar 1991</t>
+          <t>Solin</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cibalia</t>
+          <t>Orijent</t>
         </is>
       </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>2.07</v>
+        <v>2.08</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2344,7 +2344,7 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>1.98</v>
+        <v>2.05</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>3.14</v>
+        <v>3.34</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2360,7 +2360,7 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>3.32</v>
+        <v>3.65</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         </is>
       </c>
       <c r="R21" t="n">
-        <v>3.3</v>
+        <v>2.99</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>3.76</v>
+        <v>3.24</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-cibalia/Srlok6Bl/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-orijent/A7wjlQQf/</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Solin</t>
+          <t>Vukovar 1991</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Orijent</t>
+          <t>Cibalia</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>2.08</v>
+        <v>2.07</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.05</v>
+        <v>1.98</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.34</v>
+        <v>3.14</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.65</v>
+        <v>3.32</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2460,7 +2460,7 @@
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.99</v>
+        <v>3.3</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,7 +2468,7 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>3.24</v>
+        <v>3.76</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-orijent/A7wjlQQf/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-cibalia/Srlok6Bl/</t>
         </is>
       </c>
     </row>
@@ -4621,22 +4621,22 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Solin</t>
+          <t>Vukovar 1991</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Croatia Zmijavci</t>
+          <t>Dubrava</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46" t="n">
-        <v>1.89</v>
+        <v>1.61</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -4644,15 +4644,15 @@
         </is>
       </c>
       <c r="L46" t="n">
-        <v>1.79</v>
+        <v>1.84</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>30/09/2023 15:29</t>
+          <t>30/09/2023 15:15</t>
         </is>
       </c>
       <c r="N46" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -4660,15 +4660,15 @@
         </is>
       </c>
       <c r="P46" t="n">
-        <v>3.71</v>
+        <v>3.83</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>30/09/2023 15:29</t>
+          <t>30/09/2023 15:15</t>
         </is>
       </c>
       <c r="R46" t="n">
-        <v>3.41</v>
+        <v>4.43</v>
       </c>
       <c r="S46" t="inlineStr">
         <is>
@@ -4676,16 +4676,16 @@
         </is>
       </c>
       <c r="T46" t="n">
-        <v>4.1</v>
+        <v>3.75</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>30/09/2023 15:29</t>
+          <t>30/09/2023 15:15</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-croatia-zmijavci/4OeFBKOI/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-dubrava-zagreb/dbdBC09C/</t>
         </is>
       </c>
     </row>
@@ -4713,22 +4713,22 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Vukovar 1991</t>
+          <t>Solin</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Dubrava</t>
+          <t>Croatia Zmijavci</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>1.61</v>
+        <v>1.89</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -4736,15 +4736,15 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>1.84</v>
+        <v>1.79</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>30/09/2023 15:15</t>
+          <t>30/09/2023 15:29</t>
         </is>
       </c>
       <c r="N47" t="n">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4752,15 +4752,15 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>3.83</v>
+        <v>3.71</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>30/09/2023 15:15</t>
+          <t>30/09/2023 15:29</t>
         </is>
       </c>
       <c r="R47" t="n">
-        <v>4.43</v>
+        <v>3.41</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
@@ -4768,16 +4768,16 @@
         </is>
       </c>
       <c r="T47" t="n">
-        <v>3.75</v>
+        <v>4.1</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>30/09/2023 15:15</t>
+          <t>30/09/2023 15:29</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-dubrava-zagreb/dbdBC09C/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-croatia-zmijavci/4OeFBKOI/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Bijelo Brdo</t>
+          <t>Vukovar 1991</t>
         </is>
       </c>
       <c r="G82" t="n">
+        <v>2</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Orijent</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
         <v>0</v>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Sibenik</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
       <c r="J82" t="n">
-        <v>4.54</v>
+        <v>1.47</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>5.86</v>
+        <v>1.53</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>11/11/2023 13:52</t>
+          <t>11/11/2023 13:54</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.58</v>
+        <v>4.22</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>4.01</v>
+        <v>4.56</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>11/11/2023 13:52</t>
+          <t>11/11/2023 13:54</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>1.63</v>
+        <v>5.03</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>1.54</v>
+        <v>5</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>11/11/2023 13:51</t>
+          <t>11/11/2023 13:54</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/bijelo-brdo-sibenik/z5LWxIvF/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-orijent/8WYwyd9R/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Vukovar 1991</t>
+          <t>Bijelo Brdo</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Orijent</t>
+          <t>Sibenik</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>1.47</v>
+        <v>4.54</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.53</v>
+        <v>5.86</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>11/11/2023 13:54</t>
+          <t>11/11/2023 13:52</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>4.22</v>
+        <v>3.58</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>4.56</v>
+        <v>4.01</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>11/11/2023 13:54</t>
+          <t>11/11/2023 13:52</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>5.03</v>
+        <v>1.63</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>5</v>
+        <v>1.54</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>11/11/2023 13:54</t>
+          <t>11/11/2023 13:51</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-orijent/8WYwyd9R/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/bijelo-brdo-sibenik/z5LWxIvF/</t>
         </is>
       </c>
     </row>
@@ -8669,22 +8669,22 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Croatia Zmijavci</t>
+          <t>Zrinski Jurjevac</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Bijelo Brdo</t>
+          <t>Sibenik</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>1.72</v>
+        <v>2.88</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>1.63</v>
+        <v>3.22</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>19/11/2023 13:23</t>
+          <t>19/11/2023 13:27</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.47</v>
+        <v>3.08</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.41</v>
+        <v>2.68</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>19/11/2023 13:23</t>
+          <t>19/11/2023 13:27</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>4.07</v>
+        <v>2.26</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>6.12</v>
+        <v>2.58</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>19/11/2023 13:24</t>
+          <t>19/11/2023 13:27</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/croatia-zmijavci-bijelo-brdo/0UDITD11/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/zrinski-jurjevac-sibenik/0QcHlFwR/</t>
         </is>
       </c>
     </row>
@@ -8761,22 +8761,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Zrinski Jurjevac</t>
+          <t>Croatia Zmijavci</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Sibenik</t>
+          <t>Bijelo Brdo</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>2.88</v>
+        <v>1.72</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>3.22</v>
+        <v>1.63</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>19/11/2023 13:27</t>
+          <t>19/11/2023 13:23</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>3.08</v>
+        <v>3.47</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>2.68</v>
+        <v>3.41</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>19/11/2023 13:27</t>
+          <t>19/11/2023 13:23</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>2.26</v>
+        <v>4.07</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,108 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>2.58</v>
+        <v>6.12</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>19/11/2023 13:27</t>
+          <t>19/11/2023 13:24</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/zrinski-jurjevac-sibenik/0QcHlFwR/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/croatia-zmijavci-bijelo-brdo/0UDITD11/</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>croatia</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>prva-nl</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>45254.5625</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Vukovar 1991</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>3</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Sesvete</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>23/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L92" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>24/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="N92" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>23/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P92" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>24/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="R92" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>23/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T92" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="U92" t="inlineStr">
+        <is>
+          <t>24/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="V92" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/vukovar-1991-sesvete/hOxdsXV0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 27-11-2023 20:21
</commit_message>
<xml_diff>
--- a/2023/croatia_prva-nl_2023-2024.xlsx
+++ b/2023/croatia_prva-nl_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V96"/>
+  <dimension ref="A1:V97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5633,22 +5633,22 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Zrinski Jurjevac</t>
+          <t>Solin</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Croatia Zmijavci</t>
+          <t>Jarun</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>1.68</v>
+        <v>1.85</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -5656,15 +5656,15 @@
         </is>
       </c>
       <c r="L57" t="n">
-        <v>1.58</v>
+        <v>1.88</v>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>14/10/2023 14:53</t>
+          <t>14/10/2023 14:51</t>
         </is>
       </c>
       <c r="N57" t="n">
-        <v>3.61</v>
+        <v>3.54</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -5672,15 +5672,15 @@
         </is>
       </c>
       <c r="P57" t="n">
-        <v>3.86</v>
+        <v>3.62</v>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>14/10/2023 14:53</t>
+          <t>14/10/2023 14:51</t>
         </is>
       </c>
       <c r="R57" t="n">
-        <v>4.26</v>
+        <v>3.41</v>
       </c>
       <c r="S57" t="inlineStr">
         <is>
@@ -5688,16 +5688,16 @@
         </is>
       </c>
       <c r="T57" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>14/10/2023 14:53</t>
+          <t>14/10/2023 14:51</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/zrinski-jurjevac-croatia-zmijavci/dzj8RTZo/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-jarun/6BAb7QlU/</t>
         </is>
       </c>
     </row>
@@ -5725,22 +5725,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Cibalia</t>
+          <t>Zrinski Jurjevac</t>
         </is>
       </c>
       <c r="G58" t="n">
+        <v>4</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Croatia Zmijavci</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
         <v>0</v>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Sesvete</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>1</v>
-      </c>
       <c r="J58" t="n">
-        <v>1.73</v>
+        <v>1.68</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -5748,15 +5748,15 @@
         </is>
       </c>
       <c r="L58" t="n">
-        <v>1.75</v>
+        <v>1.58</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>14/10/2023 14:59</t>
+          <t>14/10/2023 14:53</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>3.53</v>
+        <v>3.61</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -5764,15 +5764,15 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>3.52</v>
+        <v>3.86</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>14/10/2023 14:59</t>
+          <t>14/10/2023 14:53</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>3.94</v>
+        <v>4.26</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
@@ -5780,16 +5780,16 @@
         </is>
       </c>
       <c r="T58" t="n">
-        <v>4.64</v>
+        <v>5.57</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>14/10/2023 14:59</t>
+          <t>14/10/2023 14:53</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/cibalia-sesvete/h2qHP74b/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/zrinski-jurjevac-croatia-zmijavci/dzj8RTZo/</t>
         </is>
       </c>
     </row>
@@ -5817,22 +5817,22 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Solin</t>
+          <t>Cibalia</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Jarun</t>
+          <t>Sesvete</t>
         </is>
       </c>
       <c r="I59" t="n">
         <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>1.85</v>
+        <v>1.73</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -5840,15 +5840,15 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>1.88</v>
+        <v>1.75</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>14/10/2023 14:51</t>
+          <t>14/10/2023 14:59</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>3.54</v>
+        <v>3.53</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5856,15 +5856,15 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>3.62</v>
+        <v>3.52</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>14/10/2023 14:51</t>
+          <t>14/10/2023 14:59</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>3.41</v>
+        <v>3.94</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
@@ -5872,16 +5872,16 @@
         </is>
       </c>
       <c r="T59" t="n">
-        <v>3.79</v>
+        <v>4.64</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>14/10/2023 14:51</t>
+          <t>14/10/2023 14:59</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/croatia/prva-nl/solin-jarun/6BAb7QlU/</t>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/cibalia-sesvete/h2qHP74b/</t>
         </is>
       </c>
     </row>
@@ -9286,6 +9286,98 @@
       <c r="V96" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/croatia/prva-nl/jarun-dugopolje/zmS0tio7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>croatia</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>prva-nl</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>45257.70833333334</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Sibenik</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>1</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Orijent</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>24/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L97" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>27/11/2023 16:58</t>
+        </is>
+      </c>
+      <c r="N97" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>24/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P97" t="n">
+        <v>6.98</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>27/11/2023 16:58</t>
+        </is>
+      </c>
+      <c r="R97" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>24/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T97" t="n">
+        <v>13.49</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>27/11/2023 16:58</t>
+        </is>
+      </c>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/croatia/prva-nl/sibenik-orijent/pbZmqg1l/</t>
         </is>
       </c>
     </row>

</xml_diff>